<commit_message>
Added and published SA 1.2-4.
</commit_message>
<xml_diff>
--- a/_data/YinshunSamyuktaAgama_PaliParallels.xlsx
+++ b/_data/YinshunSamyuktaAgama_PaliParallels.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlie\Desktop\DharmaPearls\_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlie\Desktop\The Four Agamas\_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C240C800-76F1-462D-B4B4-18DE4085BB11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D70635CE-C4B7-46E0-9753-250AA086301A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="1170" windowWidth="20640" windowHeight="15030" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Madhyama" sheetId="1" r:id="rId1"/>
@@ -9355,12 +9355,6 @@
     <t>∅</t>
   </si>
   <si>
-    <t>SN 22.13</t>
-  </si>
-  <si>
-    <t>SN 22.14</t>
-  </si>
-  <si>
     <t>SN 22.24</t>
   </si>
   <si>
@@ -9557,6 +9551,12 @@
   </si>
   <si>
     <t>MN 62, 118</t>
+  </si>
+  <si>
+    <t>SN 22.14, (22.51)</t>
+  </si>
+  <si>
+    <t>SN 22.13, (22.51)</t>
   </si>
 </sst>
 </file>
@@ -11377,7 +11377,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2342" sqref="G2342"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11466,13 +11466,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>3121</v>
+        <v>3119</v>
       </c>
       <c r="D3" s="7">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>3166</v>
+        <v>3164</v>
       </c>
       <c r="F3" t="s">
         <v>3105</v>
@@ -11492,13 +11492,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>3122</v>
+        <v>3120</v>
       </c>
       <c r="D4" s="7">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>3106</v>
+        <v>3173</v>
       </c>
       <c r="F4" t="s">
         <v>3105</v>
@@ -11518,7 +11518,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>3123</v>
+        <v>3121</v>
       </c>
       <c r="D5" s="7">
         <v>1</v>
@@ -11544,13 +11544,13 @@
         <v>1</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>3124</v>
+        <v>3122</v>
       </c>
       <c r="D6" s="7">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>3107</v>
+        <v>3172</v>
       </c>
       <c r="F6" t="s">
         <v>3105</v>
@@ -11570,7 +11570,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>3125</v>
+        <v>3123</v>
       </c>
       <c r="D7" s="7">
         <v>1</v>
@@ -11596,13 +11596,13 @@
         <v>3</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>3126</v>
+        <v>3124</v>
       </c>
       <c r="D8" s="7">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>3108</v>
+        <v>3106</v>
       </c>
       <c r="F8" t="s">
         <v>3105</v>
@@ -11622,13 +11622,13 @@
         <v>4</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>3127</v>
+        <v>3125</v>
       </c>
       <c r="D9" s="7">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>3108</v>
+        <v>3106</v>
       </c>
       <c r="F9" t="s">
         <v>3105</v>
@@ -11648,13 +11648,13 @@
         <v>5</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>3119</v>
+        <v>3117</v>
       </c>
       <c r="D10" s="7">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>3109</v>
+        <v>3107</v>
       </c>
       <c r="F10" t="s">
         <v>3105</v>
@@ -11666,7 +11666,7 @@
         <v>3105</v>
       </c>
       <c r="I10" t="s">
-        <v>3118</v>
+        <v>3116</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -11677,13 +11677,13 @@
         <v>6</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>3128</v>
+        <v>3126</v>
       </c>
       <c r="D11" s="7">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>3108</v>
+        <v>3106</v>
       </c>
       <c r="F11" t="s">
         <v>3105</v>
@@ -11703,13 +11703,13 @@
         <v>7</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>3118</v>
+        <v>3116</v>
       </c>
       <c r="D12" s="7">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>3109</v>
+        <v>3107</v>
       </c>
       <c r="F12" t="s">
         <v>3105</v>
@@ -11721,7 +11721,7 @@
         <v>3105</v>
       </c>
       <c r="I12" t="s">
-        <v>3119</v>
+        <v>3117</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -11732,13 +11732,13 @@
         <v>8</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>3129</v>
+        <v>3127</v>
       </c>
       <c r="D13" s="7">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>3110</v>
+        <v>3108</v>
       </c>
       <c r="F13" t="s">
         <v>3105</v>
@@ -11750,7 +11750,7 @@
         <v>3105</v>
       </c>
       <c r="I13" t="s">
-        <v>3120</v>
+        <v>3118</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -11761,13 +11761,13 @@
         <v>8</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>3130</v>
+        <v>3128</v>
       </c>
       <c r="D14" s="7">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>3111</v>
+        <v>3109</v>
       </c>
       <c r="F14" t="s">
         <v>3105</v>
@@ -11787,7 +11787,7 @@
         <v>8</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>3131</v>
+        <v>3129</v>
       </c>
       <c r="D15" s="7">
         <v>1</v>
@@ -11813,13 +11813,13 @@
         <v>8</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>3132</v>
+        <v>3130</v>
       </c>
       <c r="D16" s="7">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>3112</v>
+        <v>3110</v>
       </c>
       <c r="F16" t="s">
         <v>3105</v>
@@ -11839,19 +11839,19 @@
         <v>9</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>3133</v>
+        <v>3131</v>
       </c>
       <c r="D17" s="7">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>3113</v>
+        <v>3111</v>
       </c>
       <c r="F17" t="s">
         <v>3105</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>3116</v>
+        <v>3114</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>3105</v>
@@ -11865,19 +11865,19 @@
         <v>10</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>3134</v>
+        <v>3132</v>
       </c>
       <c r="D18" s="7">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>3113</v>
+        <v>3111</v>
       </c>
       <c r="F18" t="s">
         <v>3105</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>3116</v>
+        <v>3114</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>3105</v>
@@ -11891,13 +11891,13 @@
         <v>11</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>3135</v>
+        <v>3133</v>
       </c>
       <c r="D19" s="7">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>3114</v>
+        <v>3112</v>
       </c>
       <c r="F19" t="s">
         <v>3105</v>
@@ -11917,13 +11917,13 @@
         <v>12</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>3136</v>
+        <v>3134</v>
       </c>
       <c r="D20" s="7">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>3114</v>
+        <v>3112</v>
       </c>
       <c r="F20" t="s">
         <v>3105</v>
@@ -11943,7 +11943,7 @@
         <v>13</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>3137</v>
+        <v>3135</v>
       </c>
       <c r="D21" s="7">
         <v>1</v>
@@ -11969,13 +11969,13 @@
         <v>14</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>3138</v>
+        <v>3136</v>
       </c>
       <c r="D22" s="7">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>3115</v>
+        <v>3113</v>
       </c>
       <c r="F22" t="s">
         <v>3105</v>
@@ -11995,13 +11995,13 @@
         <v>15</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>3139</v>
+        <v>3137</v>
       </c>
       <c r="D23" s="7">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>3117</v>
+        <v>3115</v>
       </c>
       <c r="F23" t="s">
         <v>3105</v>
@@ -12021,13 +12021,13 @@
         <v>16</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>3140</v>
+        <v>3138</v>
       </c>
       <c r="D24" s="7">
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>3117</v>
+        <v>3115</v>
       </c>
       <c r="F24" t="s">
         <v>3105</v>
@@ -12047,7 +12047,7 @@
         <v>17</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>3141</v>
+        <v>3139</v>
       </c>
       <c r="D25" s="7">
         <v>1</v>
@@ -12073,7 +12073,7 @@
         <v>18</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>3142</v>
+        <v>3140</v>
       </c>
       <c r="D26" s="7">
         <v>1</v>
@@ -12099,7 +12099,7 @@
         <v>19</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>3144</v>
+        <v>3142</v>
       </c>
       <c r="D27" s="7">
         <v>1</v>
@@ -12125,13 +12125,13 @@
         <v>20</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>3145</v>
+        <v>3143</v>
       </c>
       <c r="D28" s="7">
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>3147</v>
+        <v>3145</v>
       </c>
       <c r="F28" t="s">
         <v>3105</v>
@@ -12151,7 +12151,7 @@
         <v>21</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>3146</v>
+        <v>3144</v>
       </c>
       <c r="D29" s="7">
         <v>1</v>
@@ -12177,7 +12177,7 @@
         <v>22</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>3148</v>
+        <v>3146</v>
       </c>
       <c r="D30" s="7">
         <v>1</v>
@@ -12203,13 +12203,13 @@
         <v>23</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>3143</v>
+        <v>3141</v>
       </c>
       <c r="D31" s="7">
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>3152</v>
+        <v>3150</v>
       </c>
       <c r="F31" t="s">
         <v>3105</v>
@@ -12221,7 +12221,7 @@
         <v>3105</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>3150</v>
+        <v>3148</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -12232,13 +12232,13 @@
         <v>24</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>3149</v>
+        <v>3147</v>
       </c>
       <c r="D32" s="7">
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>3152</v>
+        <v>3150</v>
       </c>
       <c r="F32" t="s">
         <v>3105</v>
@@ -12250,7 +12250,7 @@
         <v>3105</v>
       </c>
       <c r="I32" s="9" t="s">
-        <v>3151</v>
+        <v>3149</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -12261,13 +12261,13 @@
         <v>25</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>3153</v>
+        <v>3151</v>
       </c>
       <c r="D33" s="7">
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>3154</v>
+        <v>3152</v>
       </c>
       <c r="F33" t="s">
         <v>3105</v>
@@ -12287,13 +12287,13 @@
         <v>26</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>3155</v>
+        <v>3153</v>
       </c>
       <c r="D34" s="7">
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>3156</v>
+        <v>3154</v>
       </c>
       <c r="F34" t="s">
         <v>3105</v>
@@ -12313,13 +12313,13 @@
         <v>27</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>3158</v>
+        <v>3156</v>
       </c>
       <c r="D35" s="7">
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>3157</v>
+        <v>3155</v>
       </c>
       <c r="F35" t="s">
         <v>3105</v>
@@ -12339,13 +12339,13 @@
         <v>28</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>3160</v>
+        <v>3158</v>
       </c>
       <c r="D36" s="7">
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>3159</v>
+        <v>3157</v>
       </c>
       <c r="F36" t="s">
         <v>3105</v>
@@ -12365,13 +12365,13 @@
         <v>29</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>3161</v>
+        <v>3159</v>
       </c>
       <c r="D37" s="7">
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>3156</v>
+        <v>3154</v>
       </c>
       <c r="F37" t="s">
         <v>3105</v>
@@ -12391,7 +12391,7 @@
         <v>30</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>3163</v>
+        <v>3161</v>
       </c>
       <c r="D38" s="7">
         <v>1</v>
@@ -12417,7 +12417,7 @@
         <v>31</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>3164</v>
+        <v>3162</v>
       </c>
       <c r="D39" s="7">
         <v>1</v>
@@ -12443,13 +12443,13 @@
         <v>32</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>3165</v>
+        <v>3163</v>
       </c>
       <c r="D40" s="7">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>3162</v>
+        <v>3160</v>
       </c>
       <c r="F40" t="s">
         <v>3105</v>
@@ -15273,7 +15273,7 @@
         <v>8</v>
       </c>
       <c r="E220" t="s">
-        <v>3168</v>
+        <v>3166</v>
       </c>
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.25">
@@ -15290,7 +15290,7 @@
         <v>8</v>
       </c>
       <c r="E221" t="s">
-        <v>3169</v>
+        <v>3167</v>
       </c>
       <c r="I221" s="9" t="s">
         <v>432</v>
@@ -15415,7 +15415,7 @@
         <v>8</v>
       </c>
       <c r="E229" t="s">
-        <v>3170</v>
+        <v>3168</v>
       </c>
       <c r="I229" s="9" t="s">
         <v>433</v>
@@ -16281,7 +16281,7 @@
         <v>8</v>
       </c>
       <c r="E287" t="s">
-        <v>3171</v>
+        <v>3169</v>
       </c>
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.25">
@@ -17969,7 +17969,7 @@
         <v>11</v>
       </c>
       <c r="E399" t="s">
-        <v>3172</v>
+        <v>3170</v>
       </c>
     </row>
     <row r="400" spans="1:10" x14ac:dyDescent="0.25">
@@ -28712,7 +28712,7 @@
         <v>244</v>
       </c>
       <c r="G1086" s="5" t="s">
-        <v>3173</v>
+        <v>3171</v>
       </c>
       <c r="J1086" t="s">
         <v>247</v>
@@ -40400,7 +40400,7 @@
         <v>7</v>
       </c>
       <c r="E1856" t="s">
-        <v>3167</v>
+        <v>3165</v>
       </c>
     </row>
     <row r="1857" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Segmented and edited SA 18-23.
</commit_message>
<xml_diff>
--- a/_data/YinshunSamyuktaAgama_PaliParallels.xlsx
+++ b/_data/YinshunSamyuktaAgama_PaliParallels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlie\Desktop\DharmaPearls\_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8133E6-5142-47BC-8774-61B15ECA5757}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13E1C01-F19B-43FC-9F15-8C07F98567C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1170" windowWidth="20640" windowHeight="15030" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="20640" windowHeight="15030" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Madhyama" sheetId="1" r:id="rId1"/>
@@ -11440,8 +11440,8 @@
   <dimension ref="A1:L2457"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A972" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E994" sqref="E994"/>
+      <pane ySplit="2" topLeftCell="A975" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1026" sqref="F1026"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>